<commit_message>
Update convert_library_v2.py & README.md
- [CONTENT] (Framework) Update support for the "depends_on" field.
- [CONTENT] (Framework) Add support for the "condition" field.
TODO: Make a "example_questionnaire.xlsx" to show correctly how to make a questionnaire.
NOTE: Saved old work, working for referred questions in other requirements in "/tools/questionnaires_WIP". CAUTION: "condition" column isn't implemented in this WIP version.
- [tools] README.md: Update "depends_on" and add "condition" (Framework) descriptions
</commit_message>
<xml_diff>
--- a/tools/example_framework.xlsx
+++ b/tools/example_framework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tarkadia\projects\intuitem\ciso-assistant-community\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F2B591-24A0-474F-BEAA-028420016CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA59B32F-CADC-46F5-9032-3B98C54E3E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" tabRatio="907" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="36" windowWidth="18996" windowHeight="11136" tabRatio="907" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -405,17 +405,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Format: "line_where_the_requirement_containing_the_question_is</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>:</t>
+Format: "</t>
         </r>
         <r>
           <rPr>
@@ -467,7 +457,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{9DF94410-D1CA-448F-BD60-59EAD2557609}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{9DF94410-D1CA-448F-BD60-59EAD2557609}">
       <text>
         <r>
           <rPr>
@@ -491,7 +481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{781B3B90-5C6F-4C56-B7DD-C93B8542FECF}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{781B3B90-5C6F-4C56-B7DD-C93B8542FECF}">
       <text>
         <r>
           <rPr>
@@ -632,7 +622,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">) depends on the questions of the requirement at </t>
+          <t xml:space="preserve">) depends on the </t>
         </r>
         <r>
           <rPr>
@@ -642,16 +632,35 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Line 7 -</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">&gt; </t>
+          <t>Question 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Where is it?</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">) -&gt; </t>
         </r>
         <r>
           <rPr>
@@ -661,16 +670,16 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Question 1</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (</t>
+          <t>Choice 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> of the question (</t>
         </r>
         <r>
           <rPr>
@@ -680,45 +689,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Is the Exception respected?</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">) -&gt; </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Choice 1</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> of the question (</t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yes</t>
+          <t>A1</t>
         </r>
         <r>
           <rPr>
@@ -786,7 +757,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">) depends on the questions of the requirement at </t>
+          <t xml:space="preserve">) depends on the </t>
         </r>
         <r>
           <rPr>
@@ -796,16 +767,35 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Line 35</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> -&gt; </t>
+          <t>Question 2</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Who is it?</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">) -&gt; </t>
         </r>
         <r>
           <rPr>
@@ -815,16 +805,16 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Question 2</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (</t>
+          <t>Choice 1 or 3</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> of the question (</t>
         </r>
         <r>
           <rPr>
@@ -834,35 +824,16 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Name of 2nd department?</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">) -&gt; </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Choice 3 or 4</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> of the question (</t>
+          <t>A1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> or </t>
         </r>
         <r>
           <rPr>
@@ -872,35 +843,16 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>SUZ-DQ</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> or </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>COR-A9</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>)</t>
+          <t>C1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>).</t>
         </r>
       </text>
     </comment>
@@ -914,7 +866,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">.: Line 1,2 &amp; 3 :.
+          <t xml:space="preserve">.: Line 1 :.
 </t>
         </r>
         <r>
@@ -924,6 +876,65 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>The</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 1st Question</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Question 4?</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>) depends on nothing because a question cannot depend on itself.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+.: Line 2 &amp; 3 :.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">Means that the </t>
         </r>
         <r>
@@ -934,7 +945,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>1st, 2nd and 3rd Questions</t>
+          <t>2nd and 3rd Questions</t>
         </r>
         <r>
           <rPr>
@@ -953,6 +964,63 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Question 5?</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> and </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Question 6?</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">) depends on the </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Question 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Question 4?</t>
         </r>
         <r>
@@ -962,6 +1030,44 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">) -&gt; </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Choice 1, 2 or 3</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> of the question (</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A4</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve"> ; </t>
         </r>
         <r>
@@ -972,7 +1078,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Question 5?</t>
+          <t>B4</t>
         </r>
         <r>
           <rPr>
@@ -991,149 +1097,16 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Question 6?</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">) depends on the questions of the requirement at </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Line 5</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> -&gt; </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Question 1</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (</t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Is it true?</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">) -&gt; </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Choice 1, 2 or 3</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> of the question (</t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yes</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> ; </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>No</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> ; </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>N/A</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>)</t>
+          <t>C4</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>).</t>
         </r>
         <r>
           <rPr>
@@ -1547,7 +1520,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="688">
   <si>
     <t>type</t>
   </si>
@@ -3925,15 +3898,36 @@
 testgrp2, grp001</t>
   </si>
   <si>
+    <t>Is it true?</t>
+  </si>
+  <si>
+    <t>1:1,2,3</t>
+  </si>
+  <si>
     <t>UNDEFINED
-7:1:1
-35:2:3,4</t>
-  </si>
-  <si>
-    <t>5:1:1,2,3</t>
-  </si>
-  <si>
-    <t>Is it true?</t>
+1:1
+2:1,3</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>UNDEFINED
+any
+all</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>2:1,2
+UNDEFINED
+2:3</t>
+  </si>
+  <si>
+    <t>any
+UNDEFINED
+any</t>
   </si>
 </sst>
 </file>
@@ -4788,7 +4782,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="81">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -6101,67 +6115,68 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549B97EC-A4EC-467D-95D4-C91A5E59F559}" name="Tableau1" displayName="Tableau1" ref="A1:S51" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76" totalsRowBorderDxfId="75">
-  <autoFilter ref="A1:S51" xr:uid="{549B97EC-A4EC-467D-95D4-C91A5E59F559}"/>
-  <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{D7929412-2C04-48B2-B421-6EC19B1F374C}" name="assessable" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{BAC0F5CA-29D7-460A-BD72-3F9E24C9732F}" name="depth" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{92C5BE2B-42CA-458E-8D3C-CC37002D48BD}" name="ref_id" dataDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{9F7C5816-5FCC-476D-B6FA-AE433ADEABCC}" name="name" dataDxfId="71"/>
-    <tableColumn id="5" xr3:uid="{2650FBAE-CAA9-4751-AB1F-D901BDE6D752}" name="description" dataDxfId="70"/>
-    <tableColumn id="6" xr3:uid="{552D82DF-7C98-4797-9A2D-D4FDA52D98AF}" name="annotation" dataDxfId="69"/>
-    <tableColumn id="7" xr3:uid="{E61773D4-D778-4312-A49F-8A5758A995E8}" name="typical_evidence" dataDxfId="68"/>
-    <tableColumn id="19" xr3:uid="{DFBF3465-BE6B-4017-8F87-57A82780A75B}" name="importance" dataDxfId="67"/>
-    <tableColumn id="18" xr3:uid="{12A7028D-E894-47CA-AEF9-9E602B1E4657}" name="weight" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{41549C1C-81F1-4DC9-AF3E-D66557AB55EA}" name="implementation_groups" dataDxfId="65"/>
-    <tableColumn id="14" xr3:uid="{AFF985E6-291A-441C-8DEF-8F4448E20722}" name="questions" dataDxfId="64"/>
-    <tableColumn id="13" xr3:uid="{22C6C123-59A8-4006-974A-AEC9BDF7B9C5}" name="answer" dataDxfId="63"/>
-    <tableColumn id="17" xr3:uid="{DF10B870-B9C4-4D6A-8C84-F0105D4909E5}" name="depends_on" dataDxfId="62"/>
-    <tableColumn id="15" xr3:uid="{98B369E5-A92E-4F40-ABC5-965BF81E342E}" name="threats" dataDxfId="61"/>
-    <tableColumn id="16" xr3:uid="{12E0FCEA-DE2D-4475-972C-17BB204562B1}" name="reference_controls" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{D92464D6-5A4E-46A6-B30C-5054FBC689EF}" name="name[fr]" dataDxfId="59"/>
-    <tableColumn id="10" xr3:uid="{582EF74A-B398-41A0-ACCF-D0452C1A56EF}" name="description[fr]" dataDxfId="58"/>
-    <tableColumn id="11" xr3:uid="{EA0E2718-3825-4A77-B686-8C594E64AC01}" name="annotation[fr]" dataDxfId="57"/>
-    <tableColumn id="12" xr3:uid="{CB66FA06-DCF3-44C6-A079-7B12A457972F}" name="typical_evidence[fr]" dataDxfId="56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549B97EC-A4EC-467D-95D4-C91A5E59F559}" name="Tableau1" displayName="Tableau1" ref="A1:T51" totalsRowShown="0" headerRowDxfId="80" dataDxfId="78" headerRowBorderDxfId="79" tableBorderDxfId="77" totalsRowBorderDxfId="76">
+  <autoFilter ref="A1:T51" xr:uid="{549B97EC-A4EC-467D-95D4-C91A5E59F559}"/>
+  <tableColumns count="20">
+    <tableColumn id="1" xr3:uid="{D7929412-2C04-48B2-B421-6EC19B1F374C}" name="assessable" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{BAC0F5CA-29D7-460A-BD72-3F9E24C9732F}" name="depth" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{92C5BE2B-42CA-458E-8D3C-CC37002D48BD}" name="ref_id" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{9F7C5816-5FCC-476D-B6FA-AE433ADEABCC}" name="name" dataDxfId="72"/>
+    <tableColumn id="5" xr3:uid="{2650FBAE-CAA9-4751-AB1F-D901BDE6D752}" name="description" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{552D82DF-7C98-4797-9A2D-D4FDA52D98AF}" name="annotation" dataDxfId="70"/>
+    <tableColumn id="7" xr3:uid="{E61773D4-D778-4312-A49F-8A5758A995E8}" name="typical_evidence" dataDxfId="69"/>
+    <tableColumn id="19" xr3:uid="{DFBF3465-BE6B-4017-8F87-57A82780A75B}" name="importance" dataDxfId="68"/>
+    <tableColumn id="18" xr3:uid="{12A7028D-E894-47CA-AEF9-9E602B1E4657}" name="weight" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{41549C1C-81F1-4DC9-AF3E-D66557AB55EA}" name="implementation_groups" dataDxfId="66"/>
+    <tableColumn id="14" xr3:uid="{AFF985E6-291A-441C-8DEF-8F4448E20722}" name="questions" dataDxfId="65"/>
+    <tableColumn id="13" xr3:uid="{22C6C123-59A8-4006-974A-AEC9BDF7B9C5}" name="answer" dataDxfId="64"/>
+    <tableColumn id="17" xr3:uid="{DF10B870-B9C4-4D6A-8C84-F0105D4909E5}" name="depends_on" dataDxfId="63"/>
+    <tableColumn id="20" xr3:uid="{4DFC0890-3949-485D-8686-867538D659D0}" name="condition" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{98B369E5-A92E-4F40-ABC5-965BF81E342E}" name="threats" dataDxfId="62"/>
+    <tableColumn id="16" xr3:uid="{12E0FCEA-DE2D-4475-972C-17BB204562B1}" name="reference_controls" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{D92464D6-5A4E-46A6-B30C-5054FBC689EF}" name="name[fr]" dataDxfId="60"/>
+    <tableColumn id="10" xr3:uid="{582EF74A-B398-41A0-ACCF-D0452C1A56EF}" name="description[fr]" dataDxfId="59"/>
+    <tableColumn id="11" xr3:uid="{EA0E2718-3825-4A77-B686-8C594E64AC01}" name="annotation[fr]" dataDxfId="58"/>
+    <tableColumn id="12" xr3:uid="{CB66FA06-DCF3-44C6-A079-7B12A457972F}" name="typical_evidence[fr]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{095154CE-6DE0-439C-B5AB-1118C37DCAF4}" name="Tableau2" displayName="Tableau2" ref="A1:F8" totalsRowShown="0" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{095154CE-6DE0-439C-B5AB-1118C37DCAF4}" name="Tableau2" displayName="Tableau2" ref="A1:F8" totalsRowShown="0" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54" totalsRowBorderDxfId="53">
   <autoFilter ref="A1:F8" xr:uid="{095154CE-6DE0-439C-B5AB-1118C37DCAF4}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BB7E1ECB-4B2B-4222-B69C-FDF7FCF7F451}" name="ref_id" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{AA129DE3-6969-4BE8-8FD1-B74529AF31A8}" name="name" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{7980BF69-F795-4B15-9518-5B07FE2675D7}" name="description" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{924732DF-B0AD-42F7-8C31-80F3FDB545EE}" name="default_selected" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{245E3F68-8E07-4115-ADB2-6D2D1DB60F36}" name="name[fr]" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{7C50CF1F-76A2-4CDB-B985-67AE9549E305}" name="description[fr]" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{BB7E1ECB-4B2B-4222-B69C-FDF7FCF7F451}" name="ref_id" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{AA129DE3-6969-4BE8-8FD1-B74529AF31A8}" name="name" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{7980BF69-F795-4B15-9518-5B07FE2675D7}" name="description" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{924732DF-B0AD-42F7-8C31-80F3FDB545EE}" name="default_selected" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{245E3F68-8E07-4115-ADB2-6D2D1DB60F36}" name="name[fr]" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{7C50CF1F-76A2-4CDB-B985-67AE9549E305}" name="description[fr]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="Style de tableau 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3429E788-61C1-4DE4-9CF3-671C9CE643FD}" name="Tableau4" displayName="Tableau4" ref="A1:H32" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3429E788-61C1-4DE4-9CF3-671C9CE643FD}" name="Tableau4" displayName="Tableau4" ref="A1:H32" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="A1:H32" xr:uid="{3429E788-61C1-4DE4-9CF3-671C9CE643FD}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{162F889E-4877-4ACE-958A-41755715A824}" name="id" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{8EAFDB25-CF89-4029-A9FB-4244A3FEAF92}" name="question_type" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{6047ECFC-47B1-4CF1-856C-62F6C1E20455}" name="question_choices" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{70F917A4-A4E5-42C0-BA3B-5A06AF583DC2}" name="description" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{A4A01147-E50D-4259-A705-6F2FDEB19F26}" name="select_implementation_groups" dataDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{F9FB2847-10A0-4A69-ADCC-E8F7C6DF7416}" name="add_score" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{FFF5444F-8BD1-4B79-95F0-B652925F370E}" name="compute_result" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{46F6EBDF-F10D-485F-B69E-C9B51DF11F40}" name="color" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{162F889E-4877-4ACE-958A-41755715A824}" name="id" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{8EAFDB25-CF89-4029-A9FB-4244A3FEAF92}" name="question_type" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{6047ECFC-47B1-4CF1-856C-62F6C1E20455}" name="question_choices" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{70F917A4-A4E5-42C0-BA3B-5A06AF583DC2}" name="description" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{A4A01147-E50D-4259-A705-6F2FDEB19F26}" name="select_implementation_groups" dataDxfId="38"/>
+    <tableColumn id="9" xr3:uid="{F9FB2847-10A0-4A69-ADCC-E8F7C6DF7416}" name="add_score" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{FFF5444F-8BD1-4B79-95F0-B652925F370E}" name="compute_result" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{46F6EBDF-F10D-485F-B69E-C9B51DF11F40}" name="color" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="Style de tableau 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8AB0205B-E51F-4004-809C-4673837E5B05}" name="Tableau5" displayName="Tableau5" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8AB0205B-E51F-4004-809C-4673837E5B05}" name="Tableau5" displayName="Tableau5" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32">
   <autoFilter ref="A1:E1048576" xr:uid="{8AB0205B-E51F-4004-809C-4673837E5B05}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{881914C9-040C-42B4-91FE-05BC90988F70}" name="score"/>
@@ -6175,45 +6190,45 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{21DED0C8-7237-47BF-8873-738C4400D3DB}" name="Tableau14" displayName="Tableau14" ref="A1:G26" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{21DED0C8-7237-47BF-8873-738C4400D3DB}" name="Tableau14" displayName="Tableau14" ref="A1:G26" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="A1:G26" xr:uid="{32B00483-E3F9-4C14-B125-41886D9D0F23}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2F9E1637-D442-4022-8B78-23492F1B2FD4}" name="ref_id" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{1990900A-E9A9-4853-8F63-DC439067075E}" name="name" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{E03E16C2-E13E-458D-A24A-3C34A91E3DF2}" name="description" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{5ECFEFFA-B045-45BD-A6D7-4E11C3283380}" name="annotation" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{4F645D7B-245A-416B-9E6F-06323318E6E2}" name="name[fr]" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{E7094BA8-F77D-4F12-A3F8-7928936A0D2E}" name="description[fr]" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{B9C14FC4-B603-427E-A7F4-CACF10F7A085}" name="annotation[fr]" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{2F9E1637-D442-4022-8B78-23492F1B2FD4}" name="ref_id" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{1990900A-E9A9-4853-8F63-DC439067075E}" name="name" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{E03E16C2-E13E-458D-A24A-3C34A91E3DF2}" name="description" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{5ECFEFFA-B045-45BD-A6D7-4E11C3283380}" name="annotation" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{4F645D7B-245A-416B-9E6F-06323318E6E2}" name="name[fr]" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{E7094BA8-F77D-4F12-A3F8-7928936A0D2E}" name="description[fr]" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{B9C14FC4-B603-427E-A7F4-CACF10F7A085}" name="annotation[fr]" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="Style de tableau 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6DCAA1FD-DB86-4E15-8E31-AC99AB9F45D4}" name="Tableau3" displayName="Tableau3" ref="A1:I27" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6DCAA1FD-DB86-4E15-8E31-AC99AB9F45D4}" name="Tableau3" displayName="Tableau3" ref="A1:I27" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="A1:I27" xr:uid="{4748F8BA-F2F9-4976-90F0-1D6F9F26191B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{15A5B4EF-24CA-4813-9A39-8D55A540B838}" name="ref_id" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{541E38F3-C3CB-49DA-B177-2A1749008A5B}" name="name" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{F2BC8545-6F89-4E86-8E77-5E4AA7C0033E}" name="category" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{2D6C7622-7C26-46E8-BA06-DC874E602ECA}" name="csf_function" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{8B114798-8119-45A5-AC98-80691A7F5743}" name="description" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{3B24CD29-2024-4E6C-8EA8-A2A27F71DB45}" name="annotation" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{6D87C08C-7195-4695-A258-EC8C5FBA7769}" name="name[fr]" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{05DA7DF2-5885-4810-9061-18E2243F317E}" name="description[fr]" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{4E63784C-6489-4DCD-AFDF-2126BE436F13}" name="annotation[fr]" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{15A5B4EF-24CA-4813-9A39-8D55A540B838}" name="ref_id" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{541E38F3-C3CB-49DA-B177-2A1749008A5B}" name="name" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{F2BC8545-6F89-4E86-8E77-5E4AA7C0033E}" name="category" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{2D6C7622-7C26-46E8-BA06-DC874E602ECA}" name="csf_function" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{8B114798-8119-45A5-AC98-80691A7F5743}" name="description" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{3B24CD29-2024-4E6C-8EA8-A2A27F71DB45}" name="annotation" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{6D87C08C-7195-4695-A258-EC8C5FBA7769}" name="name[fr]" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{05DA7DF2-5885-4810-9061-18E2243F317E}" name="description[fr]" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{4E63784C-6489-4DCD-AFDF-2126BE436F13}" name="annotation[fr]" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Style de tableau 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D16BDFCB-B8D2-4F9D-906C-2230193C4279}" name="Tableau7" displayName="Tableau7" ref="A1:B4" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D16BDFCB-B8D2-4F9D-906C-2230193C4279}" name="Tableau7" displayName="Tableau7" ref="A1:B4" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:B4" xr:uid="{D16BDFCB-B8D2-4F9D-906C-2230193C4279}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{438C028E-BBB1-42A6-99B2-250AC16AFAC2}" name="prefix_id" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{A29B1659-A5F7-4CB7-96A6-4F3536BCB6B5}" name="prefix_value" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{438C028E-BBB1-42A6-99B2-250AC16AFAC2}" name="prefix_id" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{A29B1659-A5F7-4CB7-96A6-4F3536BCB6B5}" name="prefix_value" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Style de tableau 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6509,7 +6524,7 @@
   </sheetPr>
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -8827,11 +8842,11 @@
   <sheetPr codeName="Feuil4">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8848,16 +8863,18 @@
     <col min="10" max="10" width="27.44140625" style="29" customWidth="1"/>
     <col min="11" max="11" width="44.44140625" style="29" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" style="29" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" style="69" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.109375" style="69" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" style="29" customWidth="1"/>
-    <col min="17" max="17" width="31.77734375" style="29" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21" style="29" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="39.109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="12.77734375" style="29" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" style="29" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" style="69" customWidth="1"/>
+    <col min="17" max="17" width="23.109375" style="69" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5546875" style="29" customWidth="1"/>
+    <col min="19" max="19" width="31.77734375" style="29" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21" style="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="39.109375" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>31</v>
       </c>
@@ -8897,26 +8914,29 @@
       <c r="M1" s="36" t="s">
         <v>673</v>
       </c>
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="36" t="s">
+        <v>683</v>
+      </c>
+      <c r="O1" s="67" t="s">
         <v>281</v>
       </c>
-      <c r="O1" s="73" t="s">
+      <c r="P1" s="73" t="s">
         <v>391</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="S1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37"/>
       <c r="B2" s="38">
         <v>1</v>
@@ -8936,16 +8956,17 @@
       <c r="K2" s="38"/>
       <c r="L2" s="38"/>
       <c r="M2" s="38"/>
-      <c r="N2" s="39"/>
+      <c r="N2" s="38"/>
       <c r="O2" s="39"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38" t="s">
+      <c r="P2" s="39"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="R2" s="38"/>
-      <c r="S2" s="40"/>
-    </row>
-    <row r="3" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S2" s="38"/>
+      <c r="T2" s="40"/>
+    </row>
+    <row r="3" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37"/>
       <c r="B3" s="38" t="s">
         <v>52</v>
@@ -8969,22 +8990,23 @@
       <c r="K3" s="38"/>
       <c r="L3" s="38"/>
       <c r="M3" s="38"/>
-      <c r="N3" s="39"/>
+      <c r="N3" s="38"/>
       <c r="O3" s="39"/>
-      <c r="P3" s="38" t="s">
+      <c r="P3" s="39"/>
+      <c r="Q3" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="Q3" s="38" t="s">
+      <c r="R3" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="R3" s="38" t="s">
+      <c r="S3" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="S3" s="38" t="s">
+      <c r="T3" s="38" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37"/>
       <c r="B4" s="38" t="s">
         <v>55</v>
@@ -9006,18 +9028,19 @@
       <c r="K4" s="38"/>
       <c r="L4" s="38"/>
       <c r="M4" s="38"/>
-      <c r="N4" s="39"/>
+      <c r="N4" s="38"/>
       <c r="O4" s="39"/>
-      <c r="P4" s="38" t="s">
+      <c r="P4" s="39"/>
+      <c r="Q4" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="Q4" s="38" t="s">
+      <c r="R4" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="38"/>
-      <c r="S4" s="40"/>
-    </row>
-    <row r="5" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S4" s="38"/>
+      <c r="T4" s="40"/>
+    </row>
+    <row r="5" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>51</v>
       </c>
@@ -9039,24 +9062,25 @@
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
       <c r="K5" s="38" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="L5" s="34" t="s">
         <v>192</v>
       </c>
       <c r="M5" s="34"/>
-      <c r="N5" s="35"/>
+      <c r="N5" s="34"/>
       <c r="O5" s="35"/>
-      <c r="P5" s="38" t="s">
+      <c r="P5" s="35"/>
+      <c r="Q5" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="Q5" s="38" t="s">
+      <c r="R5" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="R5" s="38"/>
-      <c r="S5" s="40"/>
-    </row>
-    <row r="6" spans="1:19" s="30" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="S5" s="38"/>
+      <c r="T5" s="40"/>
+    </row>
+    <row r="6" spans="1:20" s="30" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>51</v>
       </c>
@@ -9086,20 +9110,21 @@
         <v>192</v>
       </c>
       <c r="M6" s="34"/>
-      <c r="N6" s="35"/>
+      <c r="N6" s="34"/>
       <c r="O6" s="35"/>
-      <c r="P6" s="38" t="s">
+      <c r="P6" s="35"/>
+      <c r="Q6" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="Q6" s="38" t="s">
+      <c r="R6" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="R6" s="38" t="s">
+      <c r="S6" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="S6" s="40"/>
-    </row>
-    <row r="7" spans="1:19" s="30" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T6" s="40"/>
+    </row>
+    <row r="7" spans="1:20" s="30" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>51</v>
       </c>
@@ -9129,18 +9154,19 @@
       <c r="M7" s="39"/>
       <c r="N7" s="39"/>
       <c r="O7" s="39"/>
-      <c r="P7" s="38" t="s">
+      <c r="P7" s="39"/>
+      <c r="Q7" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="Q7" s="38" t="s">
+      <c r="R7" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38" t="s">
+      <c r="S7" s="38"/>
+      <c r="T7" s="38" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
         <v>51</v>
       </c>
@@ -9166,22 +9192,23 @@
       <c r="K8" s="38"/>
       <c r="L8" s="38"/>
       <c r="M8" s="38"/>
-      <c r="N8" s="39"/>
+      <c r="N8" s="38"/>
       <c r="O8" s="39"/>
-      <c r="P8" s="38" t="s">
+      <c r="P8" s="39"/>
+      <c r="Q8" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="Q8" s="38" t="s">
+      <c r="R8" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="R8" s="38" t="s">
+      <c r="S8" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="S8" s="38" t="s">
+      <c r="T8" s="38" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
         <v>51</v>
       </c>
@@ -9203,16 +9230,17 @@
       <c r="K9" s="38"/>
       <c r="L9" s="38"/>
       <c r="M9" s="38"/>
-      <c r="N9" s="39"/>
+      <c r="N9" s="38"/>
       <c r="O9" s="39"/>
-      <c r="P9" s="38" t="s">
+      <c r="P9" s="39"/>
+      <c r="Q9" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="Q9" s="38"/>
       <c r="R9" s="38"/>
-      <c r="S9" s="40"/>
-    </row>
-    <row r="10" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S9" s="38"/>
+      <c r="T9" s="40"/>
+    </row>
+    <row r="10" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
         <v>51</v>
       </c>
@@ -9232,16 +9260,17 @@
       <c r="K10" s="38"/>
       <c r="L10" s="38"/>
       <c r="M10" s="38"/>
-      <c r="N10" s="39"/>
+      <c r="N10" s="38"/>
       <c r="O10" s="39"/>
-      <c r="P10" s="38" t="s">
+      <c r="P10" s="39"/>
+      <c r="Q10" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="Q10" s="38"/>
       <c r="R10" s="38"/>
-      <c r="S10" s="40"/>
-    </row>
-    <row r="11" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S10" s="38"/>
+      <c r="T10" s="40"/>
+    </row>
+    <row r="11" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
         <v>51</v>
       </c>
@@ -9265,18 +9294,19 @@
       <c r="K11" s="38"/>
       <c r="L11" s="38"/>
       <c r="M11" s="38"/>
-      <c r="N11" s="39"/>
+      <c r="N11" s="38"/>
       <c r="O11" s="39"/>
-      <c r="P11" s="38" t="s">
+      <c r="P11" s="39"/>
+      <c r="Q11" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="Q11" s="38" t="s">
+      <c r="R11" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="R11" s="38"/>
-      <c r="S11" s="40"/>
-    </row>
-    <row r="12" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S11" s="38"/>
+      <c r="T11" s="40"/>
+    </row>
+    <row r="12" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="37" t="s">
         <v>51</v>
       </c>
@@ -9298,18 +9328,19 @@
       <c r="K12" s="38"/>
       <c r="L12" s="38"/>
       <c r="M12" s="38"/>
-      <c r="N12" s="39"/>
+      <c r="N12" s="38"/>
       <c r="O12" s="39"/>
-      <c r="P12" s="38" t="s">
+      <c r="P12" s="39"/>
+      <c r="Q12" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="Q12" s="38" t="s">
+      <c r="R12" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="R12" s="38"/>
-      <c r="S12" s="40"/>
-    </row>
-    <row r="13" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S12" s="38"/>
+      <c r="T12" s="40"/>
+    </row>
+    <row r="13" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
         <v>51</v>
       </c>
@@ -9333,18 +9364,19 @@
       <c r="K13" s="38"/>
       <c r="L13" s="38"/>
       <c r="M13" s="38"/>
-      <c r="N13" s="39"/>
+      <c r="N13" s="38"/>
       <c r="O13" s="39"/>
-      <c r="P13" s="38" t="s">
+      <c r="P13" s="39"/>
+      <c r="Q13" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="Q13" s="38" t="s">
+      <c r="R13" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="R13" s="38"/>
-      <c r="S13" s="40"/>
-    </row>
-    <row r="14" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S13" s="38"/>
+      <c r="T13" s="40"/>
+    </row>
+    <row r="14" spans="1:20" s="30" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="37"/>
       <c r="B14" s="38" t="s">
         <v>57</v>
@@ -9362,18 +9394,19 @@
       <c r="K14" s="38"/>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39" t="s">
+      <c r="N14" s="38"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39" t="s">
         <v>531</v>
       </c>
-      <c r="P14" s="38" t="s">
+      <c r="Q14" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="Q14" s="38"/>
       <c r="R14" s="38"/>
-      <c r="S14" s="40"/>
-    </row>
-    <row r="15" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S14" s="38"/>
+      <c r="T14" s="40"/>
+    </row>
+    <row r="15" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>51</v>
       </c>
@@ -9401,20 +9434,21 @@
       <c r="K15" s="17"/>
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="68"/>
-      <c r="O15" s="74" t="s">
+      <c r="N15" s="17"/>
+      <c r="O15" s="68"/>
+      <c r="P15" s="74" t="s">
         <v>529</v>
       </c>
-      <c r="P15" s="38" t="s">
+      <c r="Q15" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="38" t="s">
+      <c r="R15" s="38"/>
+      <c r="S15" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="S15" s="40"/>
-    </row>
-    <row r="16" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T15" s="40"/>
+    </row>
+    <row r="16" spans="1:20" s="30" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>51</v>
       </c>
@@ -9442,20 +9476,21 @@
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
-      <c r="N16" s="68"/>
-      <c r="O16" s="68" t="s">
+      <c r="N16" s="17"/>
+      <c r="O16" s="68"/>
+      <c r="P16" s="68" t="s">
         <v>530</v>
       </c>
-      <c r="P16" s="38" t="s">
+      <c r="Q16" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="Q16" s="38"/>
       <c r="R16" s="38"/>
-      <c r="S16" s="38" t="s">
+      <c r="S16" s="38"/>
+      <c r="T16" s="38" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="30" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" s="30" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
         <v>51</v>
       </c>
@@ -9483,22 +9518,23 @@
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
-      <c r="N17" s="68"/>
-      <c r="O17" s="68" t="s">
+      <c r="N17" s="17"/>
+      <c r="O17" s="68"/>
+      <c r="P17" s="68" t="s">
         <v>532</v>
       </c>
-      <c r="P17" s="38" t="s">
+      <c r="Q17" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38" t="s">
+      <c r="R17" s="38"/>
+      <c r="S17" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="S17" s="38" t="s">
+      <c r="T17" s="38" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="30" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="37" t="s">
         <v>51</v>
       </c>
@@ -9522,18 +9558,19 @@
       <c r="K18" s="38"/>
       <c r="L18" s="38"/>
       <c r="M18" s="38"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="68" t="s">
+      <c r="N18" s="38"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="68" t="s">
         <v>533</v>
       </c>
-      <c r="P18" s="38" t="s">
+      <c r="Q18" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="Q18" s="38"/>
       <c r="R18" s="38"/>
-      <c r="S18" s="40"/>
-    </row>
-    <row r="19" spans="1:19" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="S18" s="38"/>
+      <c r="T18" s="40"/>
+    </row>
+    <row r="19" spans="1:20" s="30" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
         <v>51</v>
       </c>
@@ -9557,20 +9594,21 @@
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
       <c r="M19" s="24"/>
-      <c r="N19" s="43" t="s">
+      <c r="N19" s="24"/>
+      <c r="O19" s="43" t="s">
         <v>534</v>
       </c>
-      <c r="O19" s="68" t="s">
+      <c r="P19" s="68" t="s">
         <v>535</v>
       </c>
-      <c r="P19" s="38" t="s">
+      <c r="Q19" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="Q19" s="38"/>
       <c r="R19" s="38"/>
-      <c r="S19" s="40"/>
-    </row>
-    <row r="20" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S19" s="38"/>
+      <c r="T19" s="40"/>
+    </row>
+    <row r="20" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>51</v>
       </c>
@@ -9594,18 +9632,19 @@
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
-      <c r="N20" s="68"/>
-      <c r="O20" s="68" t="s">
+      <c r="N20" s="17"/>
+      <c r="O20" s="68"/>
+      <c r="P20" s="68" t="s">
         <v>541</v>
       </c>
-      <c r="P20" s="38" t="s">
+      <c r="Q20" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="Q20" s="38"/>
       <c r="R20" s="38"/>
-      <c r="S20" s="40"/>
-    </row>
-    <row r="21" spans="1:19" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="S20" s="38"/>
+      <c r="T20" s="40"/>
+    </row>
+    <row r="21" spans="1:20" s="30" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>51</v>
       </c>
@@ -9625,18 +9664,19 @@
       <c r="K21" s="38"/>
       <c r="L21" s="38"/>
       <c r="M21" s="38"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39" t="s">
+      <c r="N21" s="38"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39" t="s">
         <v>542</v>
       </c>
-      <c r="P21" s="38" t="s">
+      <c r="Q21" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="Q21" s="38"/>
       <c r="R21" s="38"/>
-      <c r="S21" s="40"/>
-    </row>
-    <row r="22" spans="1:19" s="30" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="S21" s="38"/>
+      <c r="T21" s="40"/>
+    </row>
+    <row r="22" spans="1:20" s="30" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="37"/>
       <c r="B22" s="38" t="s">
         <v>68</v>
@@ -9658,20 +9698,21 @@
       <c r="K22" s="38"/>
       <c r="L22" s="38"/>
       <c r="M22" s="38"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="39" t="s">
+      <c r="N22" s="38"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="39" t="s">
         <v>544</v>
       </c>
-      <c r="P22" s="38" t="s">
+      <c r="Q22" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="Q22" s="38" t="s">
+      <c r="R22" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="R22" s="38"/>
-      <c r="S22" s="40"/>
-    </row>
-    <row r="23" spans="1:19" s="30" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="S22" s="38"/>
+      <c r="T22" s="40"/>
+    </row>
+    <row r="23" spans="1:20" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>51</v>
       </c>
@@ -9691,20 +9732,21 @@
       <c r="K23" s="38"/>
       <c r="L23" s="38"/>
       <c r="M23" s="38"/>
-      <c r="N23" s="39" t="s">
+      <c r="N23" s="38"/>
+      <c r="O23" s="39" t="s">
         <v>380</v>
       </c>
-      <c r="O23" s="39" t="s">
+      <c r="P23" s="39" t="s">
         <v>543</v>
       </c>
-      <c r="P23" s="38" t="s">
+      <c r="Q23" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="Q23" s="38"/>
       <c r="R23" s="38"/>
-      <c r="S23" s="40"/>
-    </row>
-    <row r="24" spans="1:19" s="30" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="S23" s="38"/>
+      <c r="T23" s="40"/>
+    </row>
+    <row r="24" spans="1:20" s="30" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A24" s="37" t="s">
         <v>51</v>
       </c>
@@ -9724,18 +9766,19 @@
       <c r="K24" s="38"/>
       <c r="L24" s="38"/>
       <c r="M24" s="38"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39" t="s">
+      <c r="N24" s="38"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39" t="s">
         <v>545</v>
       </c>
-      <c r="P24" s="38" t="s">
+      <c r="Q24" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="Q24" s="38"/>
       <c r="R24" s="38"/>
-      <c r="S24" s="40"/>
-    </row>
-    <row r="25" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S24" s="38"/>
+      <c r="T24" s="40"/>
+    </row>
+    <row r="25" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37" t="s">
         <v>51</v>
       </c>
@@ -9757,16 +9800,17 @@
       <c r="K25" s="38"/>
       <c r="L25" s="38"/>
       <c r="M25" s="38"/>
-      <c r="N25" s="39"/>
+      <c r="N25" s="38"/>
       <c r="O25" s="39"/>
-      <c r="P25" s="38" t="s">
+      <c r="P25" s="39"/>
+      <c r="Q25" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="Q25" s="38"/>
       <c r="R25" s="38"/>
-      <c r="S25" s="40"/>
-    </row>
-    <row r="26" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S25" s="38"/>
+      <c r="T25" s="40"/>
+    </row>
+    <row r="26" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
         <v>51</v>
       </c>
@@ -9788,16 +9832,17 @@
       <c r="K26" s="38"/>
       <c r="L26" s="38"/>
       <c r="M26" s="38"/>
-      <c r="N26" s="39"/>
+      <c r="N26" s="38"/>
       <c r="O26" s="39"/>
-      <c r="P26" s="38" t="s">
+      <c r="P26" s="39"/>
+      <c r="Q26" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="Q26" s="38"/>
       <c r="R26" s="38"/>
-      <c r="S26" s="40"/>
-    </row>
-    <row r="27" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S26" s="38"/>
+      <c r="T26" s="40"/>
+    </row>
+    <row r="27" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>51</v>
       </c>
@@ -9819,16 +9864,17 @@
       <c r="K27" s="38"/>
       <c r="L27" s="38"/>
       <c r="M27" s="38"/>
-      <c r="N27" s="39"/>
+      <c r="N27" s="38"/>
       <c r="O27" s="39"/>
-      <c r="P27" s="38" t="s">
+      <c r="P27" s="39"/>
+      <c r="Q27" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="Q27" s="38"/>
       <c r="R27" s="38"/>
-      <c r="S27" s="40"/>
-    </row>
-    <row r="28" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S27" s="38"/>
+      <c r="T27" s="40"/>
+    </row>
+    <row r="28" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
       <c r="B28" s="38" t="s">
         <v>55</v>
@@ -9848,18 +9894,19 @@
       <c r="K28" s="38"/>
       <c r="L28" s="38"/>
       <c r="M28" s="38"/>
-      <c r="N28" s="39"/>
+      <c r="N28" s="38"/>
       <c r="O28" s="39"/>
-      <c r="P28" s="38" t="s">
+      <c r="P28" s="39"/>
+      <c r="Q28" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="Q28" s="38" t="s">
+      <c r="R28" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="R28" s="38"/>
-      <c r="S28" s="40"/>
-    </row>
-    <row r="29" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S28" s="38"/>
+      <c r="T28" s="40"/>
+    </row>
+    <row r="29" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="37"/>
       <c r="B29" s="38" t="s">
         <v>55</v>
@@ -9881,18 +9928,19 @@
       <c r="K29" s="38"/>
       <c r="L29" s="38"/>
       <c r="M29" s="38"/>
-      <c r="N29" s="39"/>
+      <c r="N29" s="38"/>
       <c r="O29" s="39"/>
-      <c r="P29" s="38" t="s">
+      <c r="P29" s="39"/>
+      <c r="Q29" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="Q29" s="38" t="s">
+      <c r="R29" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="R29" s="38"/>
-      <c r="S29" s="40"/>
-    </row>
-    <row r="30" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S29" s="38"/>
+      <c r="T29" s="40"/>
+    </row>
+    <row r="30" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="37"/>
       <c r="B30" s="38" t="s">
         <v>55</v>
@@ -9914,20 +9962,21 @@
       <c r="K30" s="38"/>
       <c r="L30" s="38"/>
       <c r="M30" s="38"/>
-      <c r="N30" s="39" t="s">
+      <c r="N30" s="38"/>
+      <c r="O30" s="39" t="s">
         <v>377</v>
       </c>
-      <c r="O30" s="39"/>
-      <c r="P30" s="38" t="s">
+      <c r="P30" s="39"/>
+      <c r="Q30" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="Q30" s="38" t="s">
+      <c r="R30" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="R30" s="38"/>
-      <c r="S30" s="40"/>
-    </row>
-    <row r="31" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S30" s="38"/>
+      <c r="T30" s="40"/>
+    </row>
+    <row r="31" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="41"/>
       <c r="B31" s="42" t="s">
         <v>55</v>
@@ -9949,20 +9998,21 @@
       <c r="K31" s="42"/>
       <c r="L31" s="42"/>
       <c r="M31" s="42"/>
-      <c r="N31" s="43" t="s">
+      <c r="N31" s="42"/>
+      <c r="O31" s="43" t="s">
         <v>378</v>
       </c>
-      <c r="O31" s="43"/>
-      <c r="P31" s="42" t="s">
+      <c r="P31" s="43"/>
+      <c r="Q31" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="Q31" s="38" t="s">
+      <c r="R31" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="R31" s="42"/>
-      <c r="S31" s="70"/>
-    </row>
-    <row r="32" spans="1:19" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="S31" s="42"/>
+      <c r="T31" s="70"/>
+    </row>
+    <row r="32" spans="1:20" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="41"/>
       <c r="B32" s="42" t="s">
         <v>5</v>
@@ -9980,18 +10030,19 @@
       <c r="K32" s="42"/>
       <c r="L32" s="42"/>
       <c r="M32" s="42"/>
-      <c r="N32" s="43" t="s">
+      <c r="N32" s="42"/>
+      <c r="O32" s="43" t="s">
         <v>379</v>
       </c>
-      <c r="O32" s="43"/>
-      <c r="P32" s="42" t="s">
+      <c r="P32" s="43"/>
+      <c r="Q32" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="Q32" s="42"/>
       <c r="R32" s="42"/>
-      <c r="S32" s="70"/>
-    </row>
-    <row r="33" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S32" s="42"/>
+      <c r="T32" s="70"/>
+    </row>
+    <row r="33" spans="1:21" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="41" t="s">
         <v>51</v>
       </c>
@@ -10019,20 +10070,21 @@
         <v>212</v>
       </c>
       <c r="M33" s="42"/>
-      <c r="N33" s="43" t="s">
+      <c r="N33" s="42"/>
+      <c r="O33" s="43" t="s">
         <v>380</v>
       </c>
-      <c r="O33" s="43"/>
-      <c r="P33" s="38" t="s">
+      <c r="P33" s="43"/>
+      <c r="Q33" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="Q33" s="42" t="s">
+      <c r="R33" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="R33" s="42"/>
-      <c r="S33" s="70"/>
-    </row>
-    <row r="34" spans="1:19" s="30" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="S33" s="42"/>
+      <c r="T33" s="70"/>
+    </row>
+    <row r="34" spans="1:21" s="30" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="41" t="s">
         <v>51</v>
       </c>
@@ -10062,16 +10114,17 @@
       <c r="M34" s="43"/>
       <c r="N34" s="43"/>
       <c r="O34" s="43"/>
-      <c r="P34" s="38" t="s">
+      <c r="P34" s="43"/>
+      <c r="Q34" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="Q34" s="42" t="s">
+      <c r="R34" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="R34" s="38"/>
-      <c r="S34" s="40"/>
-    </row>
-    <row r="35" spans="1:19" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="S34" s="38"/>
+      <c r="T34" s="40"/>
+    </row>
+    <row r="35" spans="1:21" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="41" t="s">
         <v>51</v>
       </c>
@@ -10097,20 +10150,21 @@
         <v>527</v>
       </c>
       <c r="M35" s="42"/>
-      <c r="N35" s="43" t="s">
+      <c r="N35" s="42"/>
+      <c r="O35" s="43" t="s">
         <v>379</v>
       </c>
-      <c r="O35" s="43"/>
-      <c r="P35" s="38" t="s">
+      <c r="P35" s="43"/>
+      <c r="Q35" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="Q35" s="42" t="s">
+      <c r="R35" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="R35" s="38"/>
-      <c r="S35" s="40"/>
-    </row>
-    <row r="36" spans="1:19" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="S35" s="38"/>
+      <c r="T35" s="40"/>
+    </row>
+    <row r="36" spans="1:21" s="30" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="41"/>
       <c r="B36" s="38" t="s">
         <v>5</v>
@@ -10128,18 +10182,19 @@
       <c r="K36" s="38"/>
       <c r="L36" s="38"/>
       <c r="M36" s="42"/>
-      <c r="N36" s="43" t="s">
+      <c r="N36" s="42"/>
+      <c r="O36" s="43" t="s">
         <v>381</v>
       </c>
-      <c r="O36" s="43"/>
-      <c r="P36" s="38" t="s">
+      <c r="P36" s="43"/>
+      <c r="Q36" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="Q36" s="38"/>
       <c r="R36" s="38"/>
-      <c r="S36" s="40"/>
-    </row>
-    <row r="37" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S36" s="38"/>
+      <c r="T36" s="40"/>
+    </row>
+    <row r="37" spans="1:21" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="41" t="s">
         <v>51</v>
       </c>
@@ -10161,20 +10216,21 @@
       <c r="K37" s="38"/>
       <c r="L37" s="38"/>
       <c r="M37" s="42"/>
-      <c r="N37" s="43" t="s">
+      <c r="N37" s="42"/>
+      <c r="O37" s="43" t="s">
         <v>382</v>
       </c>
-      <c r="O37" s="43"/>
-      <c r="P37" s="38" t="s">
+      <c r="P37" s="43"/>
+      <c r="Q37" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="Q37" s="42" t="s">
+      <c r="R37" s="42" t="s">
         <v>220</v>
       </c>
-      <c r="R37" s="38"/>
-      <c r="S37" s="40"/>
-    </row>
-    <row r="38" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S37" s="38"/>
+      <c r="T37" s="40"/>
+    </row>
+    <row r="38" spans="1:21" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="41" t="s">
         <v>51</v>
       </c>
@@ -10198,18 +10254,19 @@
       <c r="K38" s="38"/>
       <c r="L38" s="38"/>
       <c r="M38" s="38"/>
-      <c r="N38" s="39"/>
+      <c r="N38" s="38"/>
       <c r="O38" s="39"/>
-      <c r="P38" s="38" t="s">
+      <c r="P38" s="39"/>
+      <c r="Q38" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="Q38" s="42" t="s">
+      <c r="R38" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="R38" s="38"/>
-      <c r="S38" s="40"/>
-    </row>
-    <row r="39" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S38" s="38"/>
+      <c r="T38" s="40"/>
+    </row>
+    <row r="39" spans="1:21" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="41" t="s">
         <v>51</v>
       </c>
@@ -10231,18 +10288,19 @@
       <c r="K39" s="42"/>
       <c r="L39" s="42"/>
       <c r="M39" s="42"/>
-      <c r="N39" s="43"/>
+      <c r="N39" s="42"/>
       <c r="O39" s="43"/>
-      <c r="P39" s="38" t="s">
+      <c r="P39" s="43"/>
+      <c r="Q39" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="Q39" s="42" t="s">
+      <c r="R39" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="R39" s="42"/>
-      <c r="S39" s="70"/>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S39" s="42"/>
+      <c r="T39" s="70"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="37"/>
       <c r="B40" s="38" t="s">
         <v>5</v>
@@ -10262,14 +10320,16 @@
       <c r="K40" s="38"/>
       <c r="L40" s="38"/>
       <c r="M40" s="38"/>
-      <c r="N40" s="39"/>
+      <c r="N40" s="38"/>
       <c r="O40" s="39"/>
-      <c r="P40" s="38"/>
+      <c r="P40" s="39"/>
       <c r="Q40" s="38"/>
       <c r="R40" s="38"/>
-      <c r="S40" s="40"/>
-    </row>
-    <row r="41" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="S40" s="38"/>
+      <c r="T40" s="40"/>
+      <c r="U40"/>
+    </row>
+    <row r="41" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="37" t="s">
         <v>51</v>
       </c>
@@ -10293,16 +10353,20 @@
         <v>558</v>
       </c>
       <c r="M41" s="39" t="s">
-        <v>680</v>
-      </c>
-      <c r="N41" s="39"/>
+        <v>682</v>
+      </c>
+      <c r="N41" s="39" t="s">
+        <v>685</v>
+      </c>
       <c r="O41" s="39"/>
-      <c r="P41" s="38"/>
+      <c r="P41" s="39"/>
       <c r="Q41" s="38"/>
       <c r="R41" s="38"/>
-      <c r="S41" s="40"/>
-    </row>
-    <row r="42" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="S41" s="38"/>
+      <c r="T41" s="40"/>
+      <c r="U41"/>
+    </row>
+    <row r="42" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="37" t="s">
         <v>51</v>
       </c>
@@ -10328,12 +10392,14 @@
       <c r="M42" s="39"/>
       <c r="N42" s="39"/>
       <c r="O42" s="39"/>
-      <c r="P42" s="38"/>
+      <c r="P42" s="39"/>
       <c r="Q42" s="38"/>
       <c r="R42" s="38"/>
-      <c r="S42" s="40"/>
-    </row>
-    <row r="43" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="S42" s="38"/>
+      <c r="T42" s="40"/>
+      <c r="U42"/>
+    </row>
+    <row r="43" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="37" t="s">
         <v>51</v>
       </c>
@@ -10359,14 +10425,18 @@
       <c r="M43" s="39" t="s">
         <v>681</v>
       </c>
-      <c r="N43" s="39"/>
+      <c r="N43" s="39" t="s">
+        <v>684</v>
+      </c>
       <c r="O43" s="39"/>
-      <c r="P43" s="38"/>
+      <c r="P43" s="39"/>
       <c r="Q43" s="38"/>
       <c r="R43" s="38"/>
-      <c r="S43" s="40"/>
-    </row>
-    <row r="44" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="S43" s="38"/>
+      <c r="T43" s="40"/>
+      <c r="U43"/>
+    </row>
+    <row r="44" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="37" t="s">
         <v>51</v>
       </c>
@@ -10389,15 +10459,21 @@
       <c r="L44" s="39" t="s">
         <v>647</v>
       </c>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
+      <c r="M44" s="39" t="s">
+        <v>686</v>
+      </c>
+      <c r="N44" s="39" t="s">
+        <v>687</v>
+      </c>
       <c r="O44" s="39"/>
-      <c r="P44" s="38"/>
+      <c r="P44" s="39"/>
       <c r="Q44" s="38"/>
       <c r="R44" s="38"/>
-      <c r="S44" s="40"/>
-    </row>
-    <row r="45" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="S44" s="38"/>
+      <c r="T44" s="40"/>
+      <c r="U44"/>
+    </row>
+    <row r="45" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="37" t="s">
         <v>51</v>
       </c>
@@ -10423,12 +10499,14 @@
       <c r="M45" s="39"/>
       <c r="N45" s="39"/>
       <c r="O45" s="39"/>
-      <c r="P45" s="38"/>
+      <c r="P45" s="39"/>
       <c r="Q45" s="38"/>
       <c r="R45" s="38"/>
-      <c r="S45" s="40"/>
-    </row>
-    <row r="46" spans="1:19" ht="72" x14ac:dyDescent="0.3">
+      <c r="S45" s="38"/>
+      <c r="T45" s="40"/>
+      <c r="U45"/>
+    </row>
+    <row r="46" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A46" s="37" t="s">
         <v>51</v>
       </c>
@@ -10454,12 +10532,14 @@
       <c r="M46" s="39"/>
       <c r="N46" s="39"/>
       <c r="O46" s="39"/>
-      <c r="P46" s="38"/>
+      <c r="P46" s="39"/>
       <c r="Q46" s="38"/>
       <c r="R46" s="38"/>
-      <c r="S46" s="40"/>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S46" s="38"/>
+      <c r="T46" s="40"/>
+      <c r="U46"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="37" t="s">
         <v>51</v>
       </c>
@@ -10483,14 +10563,16 @@
         <v>587</v>
       </c>
       <c r="M47" s="38"/>
-      <c r="N47" s="39"/>
+      <c r="N47" s="38"/>
       <c r="O47" s="39"/>
-      <c r="P47" s="38"/>
+      <c r="P47" s="39"/>
       <c r="Q47" s="38"/>
       <c r="R47" s="38"/>
-      <c r="S47" s="40"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S47" s="38"/>
+      <c r="T47" s="40"/>
+      <c r="U47"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="37" t="s">
         <v>51</v>
       </c>
@@ -10514,14 +10596,16 @@
         <v>588</v>
       </c>
       <c r="M48" s="38"/>
-      <c r="N48" s="39"/>
+      <c r="N48" s="38"/>
       <c r="O48" s="39"/>
-      <c r="P48" s="38"/>
+      <c r="P48" s="39"/>
       <c r="Q48" s="38"/>
       <c r="R48" s="38"/>
-      <c r="S48" s="40"/>
-    </row>
-    <row r="49" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="S48" s="38"/>
+      <c r="T48" s="40"/>
+      <c r="U48"/>
+    </row>
+    <row r="49" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="37" t="s">
         <v>51</v>
       </c>
@@ -10545,14 +10629,16 @@
         <v>589</v>
       </c>
       <c r="M49" s="38"/>
-      <c r="N49" s="39"/>
+      <c r="N49" s="38"/>
       <c r="O49" s="39"/>
-      <c r="P49" s="38"/>
+      <c r="P49" s="39"/>
       <c r="Q49" s="38"/>
       <c r="R49" s="38"/>
-      <c r="S49" s="40"/>
-    </row>
-    <row r="50" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="S49" s="38"/>
+      <c r="T49" s="40"/>
+      <c r="U49"/>
+    </row>
+    <row r="50" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="37" t="s">
         <v>51</v>
       </c>
@@ -10578,12 +10664,14 @@
       <c r="M50" s="39"/>
       <c r="N50" s="39"/>
       <c r="O50" s="39"/>
-      <c r="P50" s="38"/>
+      <c r="P50" s="39"/>
       <c r="Q50" s="38"/>
       <c r="R50" s="38"/>
-      <c r="S50" s="40"/>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S50" s="38"/>
+      <c r="T50" s="40"/>
+      <c r="U50"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="37" t="s">
         <v>51</v>
       </c>
@@ -10607,12 +10695,14 @@
         <v>594</v>
       </c>
       <c r="M51" s="38"/>
-      <c r="N51" s="39"/>
+      <c r="N51" s="38"/>
       <c r="O51" s="39"/>
-      <c r="P51" s="38"/>
+      <c r="P51" s="39"/>
       <c r="Q51" s="38"/>
       <c r="R51" s="38"/>
-      <c r="S51" s="40"/>
+      <c r="S51" s="38"/>
+      <c r="T51" s="40"/>
+      <c r="U51"/>
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
@@ -10868,8 +10958,8 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update "importance" column handling
- [CONTENT] (Framework) Update support for the "importance" field (removed "undefined")
- [Script] : Update support for the "importance" field
- [tools] README.md: Update "importance" &  "default_selected" description
</commit_message>
<xml_diff>
--- a/tools/example_framework.xlsx
+++ b/tools/example_framework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tarkadia\projects\intuitem\ciso-assistant-community\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4555D90F-56C7-4C28-84D2-704721252C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B82BEC1-C307-46E4-84FF-7E6F0115A23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="907" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" tabRatio="907" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -666,7 +666,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="553">
   <si>
     <t>type</t>
   </si>
@@ -1328,9 +1328,6 @@
   </si>
   <si>
     <t>answer</t>
-  </si>
-  <si>
-    <t>Is it true ?</t>
   </si>
   <si>
     <t>Is a) respected?
@@ -2539,10 +2536,10 @@
     <t>recommended</t>
   </si>
   <si>
-    <t>undefined</t>
-  </si>
-  <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>Is it true?</t>
   </si>
 </sst>
 </file>
@@ -3003,7 +3000,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3213,11 +3210,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3228,6 +3237,69 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3252,88 +3324,7 @@
     <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4834,400 +4825,380 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="62.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="98"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="105"/>
     </row>
     <row r="2" spans="1:13" ht="42.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="99" t="s">
-        <v>545</v>
-      </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="101"/>
+      <c r="A2" s="106" t="s">
+        <v>544</v>
+      </c>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
+      <c r="K2" s="107"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="108"/>
     </row>
     <row r="3" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103"/>
-      <c r="M3" s="104"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="90"/>
     </row>
     <row r="4" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="112" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="85" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="87"/>
+    </row>
+    <row r="5" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="81" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="83"/>
-    </row>
-    <row r="5" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="92" t="s">
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="85" t="s">
+        <v>264</v>
+      </c>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="87"/>
+    </row>
+    <row r="6" spans="1:13" ht="19.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="117" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" s="117"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="85" t="s">
+        <v>265</v>
+      </c>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="87"/>
+    </row>
+    <row r="7" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="116" t="s">
+        <v>253</v>
+      </c>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="85" t="s">
+        <v>274</v>
+      </c>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="87"/>
+    </row>
+    <row r="8" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8" s="115"/>
+      <c r="C8" s="115"/>
+      <c r="D8" s="115"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="115"/>
+      <c r="G8" s="85" t="s">
+        <v>266</v>
+      </c>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="87"/>
+    </row>
+    <row r="9" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="114" t="s">
+        <v>255</v>
+      </c>
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="85" t="s">
+        <v>268</v>
+      </c>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="87"/>
+    </row>
+    <row r="10" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="109" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10" s="109"/>
+      <c r="C10" s="109"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="85" t="s">
+        <v>267</v>
+      </c>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="86"/>
+      <c r="M10" s="87"/>
+    </row>
+    <row r="11" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="110" t="s">
+        <v>272</v>
+      </c>
+      <c r="B11" s="110"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="87"/>
+    </row>
+    <row r="12" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="111" t="s">
+        <v>273</v>
+      </c>
+      <c r="B12" s="111"/>
+      <c r="C12" s="111"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="85" t="s">
+        <v>278</v>
+      </c>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="87"/>
+    </row>
+    <row r="13" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="79" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="79"/>
+      <c r="C13" s="80" t="s">
+        <v>543</v>
+      </c>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
+    </row>
+    <row r="14" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="89"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="90"/>
+    </row>
+    <row r="15" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="100" t="s">
         <v>258</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="81" t="s">
-        <v>265</v>
-      </c>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="83"/>
-    </row>
-    <row r="6" spans="1:13" ht="19.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="95" t="s">
-        <v>253</v>
-      </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="81" t="s">
-        <v>266</v>
-      </c>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="83"/>
-    </row>
-    <row r="7" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="91" t="s">
-        <v>254</v>
-      </c>
-      <c r="B7" s="91"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="91"/>
-      <c r="E7" s="91"/>
-      <c r="F7" s="91"/>
-      <c r="G7" s="81" t="s">
-        <v>275</v>
-      </c>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="83"/>
-    </row>
-    <row r="8" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="90" t="s">
-        <v>255</v>
-      </c>
-      <c r="B8" s="90"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="81" t="s">
-        <v>267</v>
-      </c>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="83"/>
-    </row>
-    <row r="9" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="89" t="s">
-        <v>256</v>
-      </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="81" t="s">
-        <v>269</v>
-      </c>
-      <c r="H9" s="82"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="82"/>
-      <c r="M9" s="83"/>
-    </row>
-    <row r="10" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="84" t="s">
-        <v>272</v>
-      </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="81" t="s">
-        <v>268</v>
-      </c>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="83"/>
-    </row>
-    <row r="11" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="85" t="s">
-        <v>273</v>
-      </c>
-      <c r="B11" s="85"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="81" t="s">
-        <v>278</v>
-      </c>
-      <c r="H11" s="82"/>
-      <c r="I11" s="82"/>
-      <c r="J11" s="82"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="82"/>
-      <c r="M11" s="83"/>
-    </row>
-    <row r="12" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="86" t="s">
-        <v>274</v>
-      </c>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="81" t="s">
-        <v>279</v>
-      </c>
-      <c r="H12" s="82"/>
-      <c r="I12" s="82"/>
-      <c r="J12" s="82"/>
-      <c r="K12" s="82"/>
-      <c r="L12" s="82"/>
-      <c r="M12" s="83"/>
-    </row>
-    <row r="13" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="105" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="105"/>
-      <c r="C13" s="106" t="s">
-        <v>544</v>
-      </c>
-      <c r="D13" s="107"/>
-      <c r="E13" s="107"/>
-      <c r="F13" s="107"/>
-      <c r="G13" s="107"/>
-      <c r="H13" s="107"/>
-      <c r="I13" s="107"/>
-      <c r="J13" s="107"/>
-      <c r="K13" s="107"/>
-      <c r="L13" s="107"/>
-      <c r="M13" s="107"/>
-    </row>
-    <row r="14" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="102" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="103"/>
-      <c r="C14" s="103"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="103"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="103"/>
-      <c r="I14" s="103"/>
-      <c r="J14" s="103"/>
-      <c r="K14" s="103"/>
-      <c r="L14" s="103"/>
-      <c r="M14" s="104"/>
-    </row>
-    <row r="15" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="117" t="s">
+      <c r="B15" s="101"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="101"/>
+      <c r="F15" s="102"/>
+      <c r="G15" s="85" t="s">
+        <v>263</v>
+      </c>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="87"/>
+    </row>
+    <row r="16" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="94" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="85" t="s">
         <v>259</v>
       </c>
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="119"/>
-      <c r="G15" s="81" t="s">
-        <v>264</v>
-      </c>
-      <c r="H15" s="82"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="82"/>
-      <c r="M15" s="83"/>
-    </row>
-    <row r="16" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="92" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="93"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="94"/>
-      <c r="G16" s="81" t="s">
+      <c r="H16" s="86"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="87"/>
+    </row>
+    <row r="17" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="97" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="98"/>
+      <c r="C17" s="98"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="99"/>
+      <c r="G17" s="85" t="s">
         <v>260</v>
       </c>
-      <c r="H16" s="82"/>
-      <c r="I16" s="82"/>
-      <c r="J16" s="82"/>
-      <c r="K16" s="82"/>
-      <c r="L16" s="82"/>
-      <c r="M16" s="83"/>
-    </row>
-    <row r="17" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="114" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="115"/>
-      <c r="C17" s="115"/>
-      <c r="D17" s="115"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="116"/>
-      <c r="G17" s="81" t="s">
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="87"/>
+    </row>
+    <row r="18" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="91" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="92"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="85" t="s">
         <v>261</v>
       </c>
-      <c r="H17" s="82"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="82"/>
-      <c r="M17" s="83"/>
-    </row>
-    <row r="18" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="111" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="112"/>
-      <c r="C18" s="112"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="113"/>
-      <c r="G18" s="81" t="s">
+      <c r="H18" s="86"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="87"/>
+    </row>
+    <row r="19" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="83"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="86"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="86"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="87"/>
+    </row>
+    <row r="20" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="79"/>
+      <c r="C20" s="80" t="s">
         <v>262</v>
       </c>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="82"/>
-      <c r="M18" s="83"/>
-    </row>
-    <row r="19" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="108" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="109"/>
-      <c r="C19" s="109"/>
-      <c r="D19" s="109"/>
-      <c r="E19" s="109"/>
-      <c r="F19" s="110"/>
-      <c r="G19" s="81" t="s">
-        <v>47</v>
-      </c>
-      <c r="H19" s="82"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="82"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="82"/>
-      <c r="M19" s="83"/>
-    </row>
-    <row r="20" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="105" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="105"/>
-      <c r="C20" s="106" t="s">
-        <v>263</v>
-      </c>
-      <c r="D20" s="107"/>
-      <c r="E20" s="107"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="107"/>
-      <c r="H20" s="107"/>
-      <c r="I20" s="107"/>
-      <c r="J20" s="107"/>
-      <c r="K20" s="107"/>
-      <c r="L20" s="107"/>
-      <c r="M20" s="107"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="81"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:M20"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="G19:M19"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:M13"/>
-    <mergeCell ref="A14:M14"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="G18:M18"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="G16:M16"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="G17:M17"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="G15:M15"/>
-    <mergeCell ref="G7:M7"/>
-    <mergeCell ref="G8:M8"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
     <mergeCell ref="G9:M9"/>
     <mergeCell ref="G12:M12"/>
     <mergeCell ref="G4:M4"/>
@@ -5244,6 +5215,26 @@
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="G5:M5"/>
     <mergeCell ref="G6:M6"/>
+    <mergeCell ref="G7:M7"/>
+    <mergeCell ref="G8:M8"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:M20"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="G19:M19"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:M13"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="G18:M18"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="G16:M16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="G17:M17"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="G15:M15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5273,7 +5264,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>10</v>
@@ -5294,16 +5285,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F2" s="47"/>
       <c r="G2" s="48"/>
@@ -5313,16 +5304,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="50" t="s">
         <v>232</v>
       </c>
-      <c r="C3" s="35" t="s">
-        <v>243</v>
-      </c>
-      <c r="D3" s="50" t="s">
-        <v>233</v>
-      </c>
       <c r="E3" s="51" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F3" s="47"/>
       <c r="G3" s="48"/>
@@ -5332,16 +5323,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="48"/>
@@ -5351,16 +5342,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="48"/>
@@ -5370,16 +5361,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F6" s="48"/>
       <c r="G6" s="48"/>
@@ -5389,16 +5380,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F7" s="48"/>
       <c r="G7" s="48"/>
@@ -5436,7 +5427,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5444,7 +5435,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -5501,559 +5492,559 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="63" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E2" s="60" t="s">
+        <v>338</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>359</v>
+      </c>
+      <c r="G2" s="31" t="s">
         <v>339</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>360</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>340</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="63" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D3" s="31"/>
       <c r="E3" s="60" t="s">
+        <v>340</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>444</v>
+      </c>
+      <c r="G3" s="31" t="s">
         <v>341</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>445</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>342</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="63" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B4" s="60" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
       <c r="E5" s="60" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="63" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B6" s="60" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
       <c r="E6" s="60" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="63" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
       <c r="E7" s="60" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="63" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B8" s="60" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="31"/>
       <c r="E8" s="60" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="63" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B9" s="60" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
       <c r="E9" s="60" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="31" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="63" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="63" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="31" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="63" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="31" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I13"/>
       <c r="J13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="63" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="63" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D15" s="31"/>
       <c r="E15" s="31" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="63" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="31" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I16"/>
       <c r="J16"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="63" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D17" s="31"/>
       <c r="E17" s="31" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="63" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D18" s="31"/>
       <c r="E18" s="31" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I18"/>
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="63" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31"/>
       <c r="E19" s="31" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="63" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B20" s="60" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E20" s="60" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="63" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B21" s="60" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D21" s="31"/>
       <c r="E21" s="60" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I21"/>
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="63" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B22" s="60" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C22" s="66"/>
       <c r="D22" s="31" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E22" s="60" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F22" s="66" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G22" s="66" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I22"/>
       <c r="J22"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="63" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B23" s="60" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C23" s="66"/>
       <c r="D23" s="66"/>
       <c r="E23" s="60" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F23" s="66" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G23" s="66" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I23"/>
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="63" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B24" s="60" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C24" s="66"/>
       <c r="D24" s="66"/>
       <c r="E24" s="60" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F24" s="66" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G24" s="66" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I24"/>
       <c r="J24"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="63" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B25" s="60" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C25" s="31"/>
       <c r="D25" s="31"/>
       <c r="E25" s="60" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I25"/>
       <c r="J25"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="63" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B26" s="60" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
       <c r="E26" s="60" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F26" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I26"/>
       <c r="J26"/>
@@ -6090,7 +6081,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6098,7 +6089,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>
@@ -6140,10 +6131,10 @@
         <v>10</v>
       </c>
       <c r="C1" s="64" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D1" s="64" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E1" s="62" t="s">
         <v>12</v>
@@ -6163,612 +6154,612 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
       <c r="E2" s="31" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
       <c r="E3" s="31" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F3" s="31"/>
       <c r="G3" s="31" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I3" s="31"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
       <c r="F4" s="31" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
       <c r="G5" s="31" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
       <c r="G6" s="31" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
       <c r="G7" s="31" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
       <c r="F8" s="31"/>
       <c r="G8" s="31" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>520</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>521</v>
-      </c>
       <c r="C9" s="31" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D9" s="66"/>
       <c r="E9" s="66"/>
       <c r="F9" s="66"/>
       <c r="G9" s="31" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H9" s="66"/>
       <c r="I9" s="66"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
+        <v>418</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>419</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>420</v>
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="31" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
       <c r="G10" s="31" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I10" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
+        <v>420</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>421</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>422</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="31" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I11" s="31" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="31" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="31" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="31" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E13" s="31"/>
       <c r="F13" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E14" s="31"/>
       <c r="F14" s="31" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="31" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F15" s="31"/>
       <c r="G15" s="31" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F16" s="31"/>
       <c r="G16" s="31" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="31" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F17" s="31"/>
       <c r="G17" s="31" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="31" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D18" s="31"/>
       <c r="E18" s="31" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F18" s="31"/>
       <c r="G18" s="31" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I18" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="31" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31"/>
       <c r="E19" s="31" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F19" s="31"/>
       <c r="G19" s="31" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H19" s="31" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H20" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I20" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F22" s="31"/>
       <c r="G22" s="31" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H22" s="31" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I22" s="31"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="31" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D23" s="31"/>
       <c r="E23" s="31"/>
       <c r="F23" s="31" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H23" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I23" s="31" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="31" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
       <c r="G24" s="31" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H24" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C25" s="31"/>
       <c r="D25" s="31"/>
       <c r="E25" s="31"/>
       <c r="F25" s="31"/>
       <c r="G25" s="31" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H25" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I25" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
       <c r="G26" s="31" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="H26" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I26" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C27" s="31"/>
       <c r="D27" s="31"/>
       <c r="E27" s="31"/>
       <c r="F27" s="31"/>
       <c r="G27" s="31" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H27" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I27" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -6802,7 +6793,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -6829,10 +6820,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
+        <v>372</v>
+      </c>
+      <c r="B1" s="68" t="s">
         <v>373</v>
-      </c>
-      <c r="B1" s="68" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6840,7 +6831,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="67" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -6848,7 +6839,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="67" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -6856,7 +6847,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="67" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -6949,7 +6940,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6970,10 +6961,10 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="78" t="s">
+        <v>535</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>536</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -7084,28 +7075,28 @@
         <v>186</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="52" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B9" s="54" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="52" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B11" s="55" t="s">
         <v>67</v>
@@ -7141,7 +7132,7 @@
   <sheetPr codeName="Feuil4">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R51"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7193,10 +7184,10 @@
         <v>33</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>547</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>548</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>34</v>
@@ -7208,10 +7199,10 @@
         <v>201</v>
       </c>
       <c r="M1" s="69" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N1" s="75" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="O1" s="14" t="s">
         <v>18</v>
@@ -7341,12 +7332,12 @@
       <c r="F5" s="40"/>
       <c r="G5" s="40"/>
       <c r="H5" s="40" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I5" s="40"/>
       <c r="J5" s="40"/>
       <c r="K5" s="40" t="s">
-        <v>202</v>
+        <v>552</v>
       </c>
       <c r="L5" s="36" t="s">
         <v>191</v>
@@ -7386,7 +7377,7 @@
       </c>
       <c r="J6" s="40"/>
       <c r="K6" s="41" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L6" s="36" t="s">
         <v>191</v>
@@ -7426,10 +7417,10 @@
       <c r="I7" s="40"/>
       <c r="J7" s="40"/>
       <c r="K7" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L7" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M7" s="41"/>
       <c r="N7" s="41"/>
@@ -7499,7 +7490,7 @@
       <c r="F9" s="40"/>
       <c r="G9" s="40"/>
       <c r="H9" s="40" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I9" s="40"/>
       <c r="J9" s="40"/>
@@ -7661,7 +7652,7 @@
       <c r="L14" s="40"/>
       <c r="M14" s="41"/>
       <c r="N14" s="41" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="O14" s="40" t="s">
         <v>139</v>
@@ -7687,7 +7678,7 @@
       </c>
       <c r="G15" s="40"/>
       <c r="H15" s="39" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I15" s="39">
         <v>5</v>
@@ -7699,7 +7690,7 @@
       <c r="L15" s="17"/>
       <c r="M15" s="70"/>
       <c r="N15" s="76" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="O15" s="40" t="s">
         <v>140</v>
@@ -7729,7 +7720,7 @@
         <v>87</v>
       </c>
       <c r="H16" s="39" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I16" s="39"/>
       <c r="J16" s="17" t="s">
@@ -7739,7 +7730,7 @@
       <c r="L16" s="17"/>
       <c r="M16" s="70"/>
       <c r="N16" s="70" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="O16" s="40" t="s">
         <v>141</v>
@@ -7779,7 +7770,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="70"/>
       <c r="N17" s="70" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="O17" s="40" t="s">
         <v>142</v>
@@ -7817,7 +7808,7 @@
       <c r="L18" s="40"/>
       <c r="M18" s="41"/>
       <c r="N18" s="70" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="O18" s="40" t="s">
         <v>143</v>
@@ -7850,10 +7841,10 @@
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
       <c r="M19" s="45" t="s">
+        <v>531</v>
+      </c>
+      <c r="N19" s="70" t="s">
         <v>532</v>
-      </c>
-      <c r="N19" s="70" t="s">
-        <v>533</v>
       </c>
       <c r="O19" s="40" t="s">
         <v>144</v>
@@ -7887,7 +7878,7 @@
       <c r="L20" s="17"/>
       <c r="M20" s="70"/>
       <c r="N20" s="70" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="O20" s="40" t="s">
         <v>145</v>
@@ -7917,7 +7908,7 @@
       <c r="L21" s="40"/>
       <c r="M21" s="41"/>
       <c r="N21" s="41" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="O21" s="40" t="s">
         <v>146</v>
@@ -7949,7 +7940,7 @@
       <c r="L22" s="40"/>
       <c r="M22" s="41"/>
       <c r="N22" s="41" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="O22" s="40" t="s">
         <v>118</v>
@@ -7980,10 +7971,10 @@
       <c r="K23" s="40"/>
       <c r="L23" s="40"/>
       <c r="M23" s="41" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="N23" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="O23" s="40" t="s">
         <v>147</v>
@@ -8013,7 +8004,7 @@
       <c r="L24" s="40"/>
       <c r="M24" s="41"/>
       <c r="N24" s="41" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="O24" s="40" t="s">
         <v>148</v>
@@ -8037,7 +8028,7 @@
       <c r="F25" s="40"/>
       <c r="G25" s="40"/>
       <c r="H25" s="40" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I25" s="40"/>
       <c r="J25" s="40"/>
@@ -8067,7 +8058,7 @@
       <c r="F26" s="40"/>
       <c r="G26" s="40"/>
       <c r="H26" s="40" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I26" s="40"/>
       <c r="J26" s="40"/>
@@ -8097,7 +8088,7 @@
       <c r="F27" s="40"/>
       <c r="G27" s="40"/>
       <c r="H27" s="40" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I27" s="40"/>
       <c r="J27" s="40"/>
@@ -8196,7 +8187,7 @@
       <c r="K30" s="40"/>
       <c r="L30" s="40"/>
       <c r="M30" s="41" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N30" s="41"/>
       <c r="O30" s="40" t="s">
@@ -8230,7 +8221,7 @@
       <c r="K31" s="44"/>
       <c r="L31" s="44"/>
       <c r="M31" s="45" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="N31" s="45"/>
       <c r="O31" s="44" t="s">
@@ -8260,7 +8251,7 @@
       <c r="K32" s="44"/>
       <c r="L32" s="44"/>
       <c r="M32" s="45" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N32" s="45"/>
       <c r="O32" s="44" t="s">
@@ -8282,30 +8273,28 @@
         <v>55</v>
       </c>
       <c r="E33" s="44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F33" s="44"/>
       <c r="G33" s="44"/>
-      <c r="H33" s="44" t="s">
-        <v>552</v>
-      </c>
+      <c r="H33" s="44"/>
       <c r="I33" s="44"/>
       <c r="J33" s="44"/>
       <c r="K33" s="44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L33" s="44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M33" s="45" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="N33" s="45"/>
       <c r="O33" s="40" t="s">
         <v>130</v>
       </c>
       <c r="P33" s="44" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q33" s="44"/>
       <c r="R33" s="72"/>
@@ -8322,7 +8311,7 @@
         <v>57</v>
       </c>
       <c r="E34" s="44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F34" s="40"/>
       <c r="G34" s="40"/>
@@ -8332,10 +8321,10 @@
       </c>
       <c r="J34" s="40"/>
       <c r="K34" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L34" s="41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M34" s="45"/>
       <c r="N34" s="45"/>
@@ -8343,7 +8332,7 @@
         <v>131</v>
       </c>
       <c r="P34" s="44" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Q34" s="40"/>
       <c r="R34" s="42"/>
@@ -8360,7 +8349,7 @@
         <v>58</v>
       </c>
       <c r="E35" s="44" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F35" s="40"/>
       <c r="G35" s="40"/>
@@ -8368,20 +8357,20 @@
       <c r="I35" s="40"/>
       <c r="J35" s="40"/>
       <c r="K35" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L35" s="40" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="M35" s="45" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N35" s="45"/>
       <c r="O35" s="40" t="s">
         <v>132</v>
       </c>
       <c r="P35" s="44" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q35" s="40"/>
       <c r="R35" s="42"/>
@@ -8404,7 +8393,7 @@
       <c r="K36" s="40"/>
       <c r="L36" s="40"/>
       <c r="M36" s="45" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="N36" s="45"/>
       <c r="O36" s="40" t="s">
@@ -8426,7 +8415,7 @@
         <v>55</v>
       </c>
       <c r="E37" s="44" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F37" s="40"/>
       <c r="G37" s="40"/>
@@ -8436,14 +8425,14 @@
       <c r="K37" s="40"/>
       <c r="L37" s="40"/>
       <c r="M37" s="45" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="N37" s="45"/>
       <c r="O37" s="40" t="s">
         <v>130</v>
       </c>
       <c r="P37" s="44" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Q37" s="40"/>
       <c r="R37" s="42"/>
@@ -8460,13 +8449,13 @@
         <v>57</v>
       </c>
       <c r="E38" s="44" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F38" s="40"/>
       <c r="G38" s="40"/>
       <c r="H38" s="40"/>
       <c r="I38" s="40" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="J38" s="40"/>
       <c r="K38" s="40"/>
@@ -8477,7 +8466,7 @@
         <v>131</v>
       </c>
       <c r="P38" s="44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q38" s="40"/>
       <c r="R38" s="42"/>
@@ -8494,7 +8483,7 @@
         <v>58</v>
       </c>
       <c r="E39" s="44" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F39" s="44"/>
       <c r="G39" s="44"/>
@@ -8509,250 +8498,10 @@
         <v>132</v>
       </c>
       <c r="P39" s="44" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q39" s="44"/>
       <c r="R39" s="72"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A40" s="79"/>
-      <c r="B40" s="79"/>
-      <c r="C40" s="79"/>
-      <c r="D40" s="79"/>
-      <c r="E40" s="79"/>
-      <c r="F40" s="79"/>
-      <c r="G40" s="79"/>
-      <c r="H40" s="79"/>
-      <c r="I40" s="79"/>
-      <c r="J40" s="79"/>
-      <c r="K40" s="79"/>
-      <c r="L40" s="79"/>
-      <c r="M40" s="80"/>
-      <c r="N40" s="80"/>
-      <c r="O40" s="79"/>
-      <c r="P40" s="79"/>
-      <c r="Q40" s="79"/>
-      <c r="R40" s="79"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A41" s="79"/>
-      <c r="B41" s="79"/>
-      <c r="C41" s="79"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="79"/>
-      <c r="F41" s="79"/>
-      <c r="G41" s="79"/>
-      <c r="H41" s="79"/>
-      <c r="I41" s="79"/>
-      <c r="J41" s="79"/>
-      <c r="K41" s="79"/>
-      <c r="L41" s="79"/>
-      <c r="M41" s="80"/>
-      <c r="N41" s="80"/>
-      <c r="O41" s="79"/>
-      <c r="P41" s="79"/>
-      <c r="Q41" s="79"/>
-      <c r="R41" s="79"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A42" s="79"/>
-      <c r="B42" s="79"/>
-      <c r="C42" s="79"/>
-      <c r="D42" s="79"/>
-      <c r="E42" s="79"/>
-      <c r="F42" s="79"/>
-      <c r="G42" s="79"/>
-      <c r="H42" s="79"/>
-      <c r="I42" s="79"/>
-      <c r="J42" s="79"/>
-      <c r="K42" s="79"/>
-      <c r="L42" s="79"/>
-      <c r="M42" s="80"/>
-      <c r="N42" s="80"/>
-      <c r="O42" s="79"/>
-      <c r="P42" s="79"/>
-      <c r="Q42" s="79"/>
-      <c r="R42" s="79"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A43" s="79"/>
-      <c r="B43" s="79"/>
-      <c r="C43" s="79"/>
-      <c r="D43" s="79"/>
-      <c r="E43" s="79"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="79"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="79"/>
-      <c r="J43" s="79"/>
-      <c r="K43" s="79"/>
-      <c r="L43" s="79"/>
-      <c r="M43" s="80"/>
-      <c r="N43" s="80"/>
-      <c r="O43" s="79"/>
-      <c r="P43" s="79"/>
-      <c r="Q43" s="79"/>
-      <c r="R43" s="79"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A44" s="79"/>
-      <c r="B44" s="79"/>
-      <c r="C44" s="79"/>
-      <c r="D44" s="79"/>
-      <c r="E44" s="79"/>
-      <c r="F44" s="79"/>
-      <c r="G44" s="79"/>
-      <c r="H44" s="79"/>
-      <c r="I44" s="79"/>
-      <c r="J44" s="79"/>
-      <c r="K44" s="79"/>
-      <c r="L44" s="79"/>
-      <c r="M44" s="80"/>
-      <c r="N44" s="80"/>
-      <c r="O44" s="79"/>
-      <c r="P44" s="79"/>
-      <c r="Q44" s="79"/>
-      <c r="R44" s="79"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A45" s="79"/>
-      <c r="B45" s="79"/>
-      <c r="C45" s="79"/>
-      <c r="D45" s="79"/>
-      <c r="E45" s="79"/>
-      <c r="F45" s="79"/>
-      <c r="G45" s="79"/>
-      <c r="H45" s="79"/>
-      <c r="I45" s="79"/>
-      <c r="J45" s="79"/>
-      <c r="K45" s="79"/>
-      <c r="L45" s="79"/>
-      <c r="M45" s="80"/>
-      <c r="N45" s="80"/>
-      <c r="O45" s="79"/>
-      <c r="P45" s="79"/>
-      <c r="Q45" s="79"/>
-      <c r="R45" s="79"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A46" s="79"/>
-      <c r="B46" s="79"/>
-      <c r="C46" s="79"/>
-      <c r="D46" s="79"/>
-      <c r="E46" s="79"/>
-      <c r="F46" s="79"/>
-      <c r="G46" s="79"/>
-      <c r="H46" s="79"/>
-      <c r="I46" s="79"/>
-      <c r="J46" s="79"/>
-      <c r="K46" s="79"/>
-      <c r="L46" s="79"/>
-      <c r="M46" s="80"/>
-      <c r="N46" s="80"/>
-      <c r="O46" s="79"/>
-      <c r="P46" s="79"/>
-      <c r="Q46" s="79"/>
-      <c r="R46" s="79"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A47" s="79"/>
-      <c r="B47" s="79"/>
-      <c r="C47" s="79"/>
-      <c r="D47" s="79"/>
-      <c r="E47" s="79"/>
-      <c r="F47" s="79"/>
-      <c r="G47" s="79"/>
-      <c r="H47" s="79"/>
-      <c r="I47" s="79"/>
-      <c r="J47" s="79"/>
-      <c r="K47" s="79"/>
-      <c r="L47" s="79"/>
-      <c r="M47" s="80"/>
-      <c r="N47" s="80"/>
-      <c r="O47" s="79"/>
-      <c r="P47" s="79"/>
-      <c r="Q47" s="79"/>
-      <c r="R47" s="79"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A48" s="79"/>
-      <c r="B48" s="79"/>
-      <c r="C48" s="79"/>
-      <c r="D48" s="79"/>
-      <c r="E48" s="79"/>
-      <c r="F48" s="79"/>
-      <c r="G48" s="79"/>
-      <c r="H48" s="79"/>
-      <c r="I48" s="79"/>
-      <c r="J48" s="79"/>
-      <c r="K48" s="79"/>
-      <c r="L48" s="79"/>
-      <c r="M48" s="80"/>
-      <c r="N48" s="80"/>
-      <c r="O48" s="79"/>
-      <c r="P48" s="79"/>
-      <c r="Q48" s="79"/>
-      <c r="R48" s="79"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A49" s="79"/>
-      <c r="B49" s="79"/>
-      <c r="C49" s="79"/>
-      <c r="D49" s="79"/>
-      <c r="E49" s="79"/>
-      <c r="F49" s="79"/>
-      <c r="G49" s="79"/>
-      <c r="H49" s="79"/>
-      <c r="I49" s="79"/>
-      <c r="J49" s="79"/>
-      <c r="K49" s="79"/>
-      <c r="L49" s="79"/>
-      <c r="M49" s="80"/>
-      <c r="N49" s="80"/>
-      <c r="O49" s="79"/>
-      <c r="P49" s="79"/>
-      <c r="Q49" s="79"/>
-      <c r="R49" s="79"/>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A50" s="79"/>
-      <c r="B50" s="79"/>
-      <c r="C50" s="79"/>
-      <c r="D50" s="79"/>
-      <c r="E50" s="79"/>
-      <c r="F50" s="79"/>
-      <c r="G50" s="79"/>
-      <c r="H50" s="79"/>
-      <c r="I50" s="79"/>
-      <c r="J50" s="79"/>
-      <c r="K50" s="79"/>
-      <c r="L50" s="79"/>
-      <c r="M50" s="80"/>
-      <c r="N50" s="80"/>
-      <c r="O50" s="79"/>
-      <c r="P50" s="79"/>
-      <c r="Q50" s="79"/>
-      <c r="R50" s="79"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A51" s="79"/>
-      <c r="B51" s="79"/>
-      <c r="C51" s="79"/>
-      <c r="D51" s="79"/>
-      <c r="E51" s="79"/>
-      <c r="F51" s="79"/>
-      <c r="G51" s="79"/>
-      <c r="H51" s="79"/>
-      <c r="I51" s="79"/>
-      <c r="J51" s="79"/>
-      <c r="K51" s="79"/>
-      <c r="L51" s="79"/>
-      <c r="M51" s="80"/>
-      <c r="N51" s="80"/>
-      <c r="O51" s="79"/>
-      <c r="P51" s="79"/>
-      <c r="Q51" s="79"/>
-      <c r="R51" s="79"/>
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
@@ -8941,7 +8690,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -8995,7 +8744,7 @@
         <v>198</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C3" s="35" t="s">
         <v>199</v>
@@ -9003,24 +8752,24 @@
     </row>
     <row r="4" spans="1:3" s="30" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" s="35" t="s">
         <v>212</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="30" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>192</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -9068,7 +8817,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -9076,7 +8825,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(tool): Add Label Integration (Update convert_library_v2.py) (#2891)
* Add Label Support

- Added label parsing logic
- [tools] README.md: Added "labels" field description
- Added "labels" field example in "example_framework.xlsx"

* Fix typo in README.md

* Fix for CodeFactor

* Fix Typos & Update Label Verification

* Merge branch 'main' into CA-1392-Add-Label-integration-to-convert_library_v2.py

* Make code more pythonic

* avoid duplicate / fix NIS2 lib

* Update README.md

---------

Co-authored-by: eric-intuitem <71850047+eric-intuitem@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tools/example_framework.xlsx
+++ b/tools/example_framework.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tarkadia\projects\intuitem\ciso-assistant-community\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E84F6D-1951-4647-B96B-120B76A95CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1C6024-1613-47E4-AAEF-428390C867CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" tabRatio="907" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{8377CD80-173C-4910-ABAF-16B301C42544}">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{FCDB3F77-8B06-4998-BCDC-B60DCE09EC36}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">.: About label :.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Works like the hashtag system in social media. Labels mustn't contains spaces. They are  separated by line breaks or commas.
+All labels will be forced to uppercase in the resulting YAML file.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{8377CD80-173C-4910-ABAF-16B301C42544}">
       <text>
         <r>
           <rPr>
@@ -666,7 +691,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="555">
   <si>
     <t>type</t>
   </si>
@@ -2541,12 +2566,18 @@
   <si>
     <t>nice_to_have</t>
   </si>
+  <si>
+    <t>labels</t>
+  </si>
+  <si>
+    <t>example_framework, framework1, my-very-cool-framework, I-LOVE-MY-FRAMEWORK</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2719,6 +2750,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="18">
@@ -3255,6 +3293,24 @@
     <xf numFmtId="0" fontId="13" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3308,24 +3364,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4825,55 +4863,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="62.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="114"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="96"/>
     </row>
     <row r="2" spans="1:13" ht="42.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="97" t="s">
         <v>544</v>
       </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="117"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="99"/>
     </row>
     <row r="3" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="96"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="102"/>
     </row>
     <row r="4" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="85" t="s">
@@ -5047,50 +5085,50 @@
       <c r="M12" s="81"/>
     </row>
     <row r="13" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="97"/>
-      <c r="C13" s="98" t="s">
+      <c r="B13" s="103"/>
+      <c r="C13" s="104" t="s">
         <v>543</v>
       </c>
-      <c r="D13" s="99"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="99"/>
-      <c r="J13" s="99"/>
-      <c r="K13" s="99"/>
-      <c r="L13" s="99"/>
-      <c r="M13" s="99"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
+      <c r="K13" s="105"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
     </row>
     <row r="14" spans="1:13" ht="34.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="95"/>
-      <c r="C14" s="95"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="95"/>
-      <c r="F14" s="95"/>
-      <c r="G14" s="95"/>
-      <c r="H14" s="95"/>
-      <c r="I14" s="95"/>
-      <c r="J14" s="95"/>
-      <c r="K14" s="95"/>
-      <c r="L14" s="95"/>
-      <c r="M14" s="96"/>
+      <c r="B14" s="101"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="101"/>
+      <c r="F14" s="101"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="101"/>
+      <c r="J14" s="101"/>
+      <c r="K14" s="101"/>
+      <c r="L14" s="101"/>
+      <c r="M14" s="102"/>
     </row>
     <row r="15" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="109" t="s">
+      <c r="A15" s="115" t="s">
         <v>258</v>
       </c>
-      <c r="B15" s="110"/>
-      <c r="C15" s="110"/>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="111"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="117"/>
       <c r="G15" s="79" t="s">
         <v>263</v>
       </c>
@@ -5121,14 +5159,14 @@
       <c r="M16" s="81"/>
     </row>
     <row r="17" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="106" t="s">
+      <c r="A17" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="107"/>
-      <c r="C17" s="107"/>
-      <c r="D17" s="107"/>
-      <c r="E17" s="107"/>
-      <c r="F17" s="108"/>
+      <c r="B17" s="113"/>
+      <c r="C17" s="113"/>
+      <c r="D17" s="113"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="114"/>
       <c r="G17" s="79" t="s">
         <v>260</v>
       </c>
@@ -5140,14 +5178,14 @@
       <c r="M17" s="81"/>
     </row>
     <row r="18" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="103" t="s">
+      <c r="A18" s="109" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="104"/>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="105"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="110"/>
+      <c r="D18" s="110"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="111"/>
       <c r="G18" s="79" t="s">
         <v>261</v>
       </c>
@@ -5159,14 +5197,14 @@
       <c r="M18" s="81"/>
     </row>
     <row r="19" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="100" t="s">
+      <c r="A19" s="106" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="101"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="102"/>
+      <c r="B19" s="107"/>
+      <c r="C19" s="107"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="108"/>
       <c r="G19" s="79" t="s">
         <v>47</v>
       </c>
@@ -5178,23 +5216,23 @@
       <c r="M19" s="81"/>
     </row>
     <row r="20" spans="1:13" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="97" t="s">
+      <c r="A20" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="97"/>
-      <c r="C20" s="98" t="s">
+      <c r="B20" s="103"/>
+      <c r="C20" s="104" t="s">
         <v>262</v>
       </c>
-      <c r="D20" s="99"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="99"/>
-      <c r="I20" s="99"/>
-      <c r="J20" s="99"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="99"/>
-      <c r="M20" s="99"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="105"/>
+      <c r="G20" s="105"/>
+      <c r="H20" s="105"/>
+      <c r="I20" s="105"/>
+      <c r="J20" s="105"/>
+      <c r="K20" s="105"/>
+      <c r="L20" s="105"/>
+      <c r="M20" s="105"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -6867,10 +6905,10 @@
   <sheetPr codeName="Feuil2">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6961,33 +6999,41 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="78" t="s">
+        <v>553</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="78" t="s">
         <v>535</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B12" s="31" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B13" s="36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="14" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B14" s="37" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B15" s="36" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7134,9 +7180,9 @@
   </sheetPr>
   <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>